<commit_message>
Arbetar mer med iteraionsplan v1
</commit_message>
<xml_diff>
--- a/ph_product_sprint_backlog_0.03.xlsx
+++ b/ph_product_sprint_backlog_0.03.xlsx
@@ -621,10 +621,10 @@
     <t>Sätta upp arbetsmiljö</t>
   </si>
   <si>
-    <t>Arbeta med Kravspecifikation</t>
+    <t>Riskhantering, identifiera risker i projektet och Kravspecifikation</t>
   </si>
   <si>
-    <t>Riskhantering, identifiera risker i projektet</t>
+    <t>Färdigställa vision</t>
   </si>
 </sst>
 </file>
@@ -1367,6 +1367,9 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1376,36 +1379,11 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="33">
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor indexed="10"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="43"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="42"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="30">
     <dxf>
       <fill>
         <patternFill>
@@ -1660,8 +1638,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.20739240506329124"/>
-          <c:y val="1.5822809259433822E-2"/>
+          <c:x val="0.20739240506329126"/>
+          <c:y val="1.5822809259433829E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:spPr>
@@ -1680,7 +1658,7 @@
           <c:x val="8.8295776413084365E-2"/>
           <c:y val="0.12658247407547046"/>
           <c:w val="0.88295776413084348"/>
-          <c:h val="0.76582396815659681"/>
+          <c:h val="0.76582396815659692"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -1973,11 +1951,11 @@
           </c:downBars>
         </c:upDownBars>
         <c:marker val="1"/>
-        <c:axId val="108272256"/>
-        <c:axId val="108282240"/>
+        <c:axId val="111823872"/>
+        <c:axId val="111833856"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="108272256"/>
+        <c:axId val="111823872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2009,7 +1987,7 @@
             <a:endParaRPr lang="sv-SE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="108282240"/>
+        <c:crossAx val="111833856"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2018,7 +1996,7 @@
         <c:tickMarkSkip val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="108282240"/>
+        <c:axId val="111833856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2060,7 +2038,7 @@
             <a:endParaRPr lang="sv-SE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="108272256"/>
+        <c:crossAx val="111823872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2108,7 +2086,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter alignWithMargins="0"/>
-    <c:pageMargins b="1" l="0.75000000000000022" r="0.75000000000000022" t="1" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1" l="0.75000000000000033" r="0.75000000000000033" t="1" header="0.5" footer="0.5"/>
     <c:pageSetup paperSize="9" orientation="landscape"/>
   </c:printSettings>
 </c:chartSpace>
@@ -2165,7 +2143,7 @@
           <c:x val="9.0349166562225844E-2"/>
           <c:y val="0.13753600904370888"/>
           <c:w val="0.87885098383256044"/>
-          <c:h val="0.65043070943587378"/>
+          <c:h val="0.65043070943587389"/>
         </c:manualLayout>
       </c:layout>
       <c:barChart>
@@ -2247,8 +2225,8 @@
           </c:val>
         </c:ser>
         <c:gapWidth val="50"/>
-        <c:axId val="108313984"/>
-        <c:axId val="108332160"/>
+        <c:axId val="113119232"/>
+        <c:axId val="113120768"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -2379,11 +2357,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="108313984"/>
-        <c:axId val="108332160"/>
+        <c:axId val="113119232"/>
+        <c:axId val="113120768"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="108313984"/>
+        <c:axId val="113119232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2415,7 +2393,7 @@
             <a:endParaRPr lang="sv-SE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="108332160"/>
+        <c:crossAx val="113120768"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2424,7 +2402,7 @@
         <c:tickMarkSkip val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="108332160"/>
+        <c:axId val="113120768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2466,7 +2444,7 @@
             <a:endParaRPr lang="sv-SE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="108313984"/>
+        <c:crossAx val="113119232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2491,7 +2469,7 @@
           <c:x val="7.5975435518235393E-2"/>
           <c:y val="0.87392672413190053"/>
           <c:w val="0.852156911893721"/>
-          <c:h val="0.1060173403045256"/>
+          <c:h val="0.10601734030452559"/>
         </c:manualLayout>
       </c:layout>
       <c:spPr>
@@ -2555,7 +2533,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter alignWithMargins="0"/>
-    <c:pageMargins b="1" l="0.75000000000000022" r="0.75000000000000022" t="1" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1" l="0.75000000000000033" r="0.75000000000000033" t="1" header="0.5" footer="0.5"/>
     <c:pageSetup paperSize="9" orientation="landscape"/>
   </c:printSettings>
 </c:chartSpace>
@@ -2572,9 +2550,9 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="0.17634635691657871"/>
-          <c:y val="8.8235610910252907E-2"/>
-          <c:w val="0.81942977824709629"/>
-          <c:h val="0.83088533607154802"/>
+          <c:y val="8.8235610910252935E-2"/>
+          <c:w val="0.8194297782470964"/>
+          <c:h val="0.83088533607154813"/>
         </c:manualLayout>
       </c:layout>
       <c:barChart>
@@ -2682,8 +2660,8 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="114785664"/>
-        <c:axId val="114791552"/>
+        <c:axId val="114024448"/>
+        <c:axId val="114025984"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -2892,25 +2870,25 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="114785664"/>
-        <c:axId val="114791552"/>
+        <c:axId val="114024448"/>
+        <c:axId val="114025984"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="114785664"/>
+        <c:axId val="114024448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="1"/>
         <c:axPos val="b"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="114791552"/>
+        <c:crossAx val="114025984"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="114791552"/>
+        <c:axId val="114025984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -2944,7 +2922,7 @@
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
               <c:x val="0.1393875395987329"/>
-              <c:y val="0.1397063839412338"/>
+              <c:y val="0.13970638394123386"/>
             </c:manualLayout>
           </c:layout>
           <c:spPr>
@@ -2981,7 +2959,7 @@
             <a:endParaRPr lang="sv-SE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="114785664"/>
+        <c:crossAx val="114024448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3005,8 +2983,8 @@
           <c:yMode val="edge"/>
           <c:x val="8.4477296726504711E-3"/>
           <c:y val="6.6176708182689656E-2"/>
-          <c:w val="0.11404435058078144"/>
-          <c:h val="0.42647211939955587"/>
+          <c:w val="0.11404435058078145"/>
+          <c:h val="0.42647211939955598"/>
         </c:manualLayout>
       </c:layout>
       <c:spPr>
@@ -3070,7 +3048,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter alignWithMargins="0"/>
-    <c:pageMargins b="1" l="0.75000000000000022" r="0.75000000000000022" t="1" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1" l="0.75000000000000033" r="0.75000000000000033" t="1" header="0.5" footer="0.5"/>
     <c:pageSetup paperSize="9" orientation="landscape"/>
   </c:printSettings>
 </c:chartSpace>
@@ -3087,9 +3065,9 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="0.17634635691657871"/>
-          <c:y val="8.8235610910252962E-2"/>
-          <c:w val="0.81942977824709651"/>
-          <c:h val="0.83088533607154824"/>
+          <c:y val="8.8235610910252976E-2"/>
+          <c:w val="0.81942977824709662"/>
+          <c:h val="0.83088533607154835"/>
         </c:manualLayout>
       </c:layout>
       <c:barChart>
@@ -3197,8 +3175,8 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="131597440"/>
-        <c:axId val="131598976"/>
+        <c:axId val="117350400"/>
+        <c:axId val="117351936"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -3407,25 +3385,25 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="131597440"/>
-        <c:axId val="131598976"/>
+        <c:axId val="117350400"/>
+        <c:axId val="117351936"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="131597440"/>
+        <c:axId val="117350400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="1"/>
         <c:axPos val="b"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="131598976"/>
+        <c:crossAx val="117351936"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="131598976"/>
+        <c:axId val="117351936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -3459,7 +3437,7 @@
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
               <c:x val="0.1393875395987329"/>
-              <c:y val="0.13970638394123391"/>
+              <c:y val="0.13970638394123394"/>
             </c:manualLayout>
           </c:layout>
           <c:spPr>
@@ -3496,7 +3474,7 @@
             <a:endParaRPr lang="sv-SE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="131597440"/>
+        <c:crossAx val="117350400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3520,8 +3498,8 @@
           <c:yMode val="edge"/>
           <c:x val="8.4477296726504711E-3"/>
           <c:y val="6.6176708182689656E-2"/>
-          <c:w val="0.11404435058078147"/>
-          <c:h val="0.42647211939955609"/>
+          <c:w val="0.11404435058078148"/>
+          <c:h val="0.42647211939955626"/>
         </c:manualLayout>
       </c:layout>
       <c:spPr>
@@ -3585,7 +3563,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter alignWithMargins="0"/>
-    <c:pageMargins b="1" l="0.75000000000000044" r="0.75000000000000044" t="1" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1" l="0.75000000000000056" r="0.75000000000000056" t="1" header="0.5" footer="0.5"/>
     <c:pageSetup paperSize="9" orientation="landscape"/>
   </c:printSettings>
 </c:chartSpace>
@@ -3601,10 +3579,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.17845828933474134"/>
-          <c:y val="8.8235610910252907E-2"/>
-          <c:w val="0.8173178458289333"/>
-          <c:h val="0.83088533607154802"/>
+          <c:x val="0.17845828933474137"/>
+          <c:y val="8.8235610910252935E-2"/>
+          <c:w val="0.81731784582893319"/>
+          <c:h val="0.83088533607154813"/>
         </c:manualLayout>
       </c:layout>
       <c:barChart>
@@ -3712,8 +3690,8 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="116104576"/>
-        <c:axId val="116110464"/>
+        <c:axId val="116748288"/>
+        <c:axId val="116749824"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -3922,25 +3900,25 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="116104576"/>
-        <c:axId val="116110464"/>
+        <c:axId val="116748288"/>
+        <c:axId val="116749824"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="116104576"/>
+        <c:axId val="116748288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="1"/>
         <c:axPos val="b"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="116110464"/>
+        <c:crossAx val="116749824"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="116110464"/>
+        <c:axId val="116749824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -3974,7 +3952,7 @@
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
               <c:x val="0.1393875395987329"/>
-              <c:y val="0.1397063839412338"/>
+              <c:y val="0.13970638394123386"/>
             </c:manualLayout>
           </c:layout>
           <c:spPr>
@@ -4011,7 +3989,7 @@
             <a:endParaRPr lang="sv-SE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="116104576"/>
+        <c:crossAx val="116748288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4035,8 +4013,8 @@
           <c:yMode val="edge"/>
           <c:x val="8.4477296726504711E-3"/>
           <c:y val="6.6176708182689656E-2"/>
-          <c:w val="0.11404435058078144"/>
-          <c:h val="0.42647211939955587"/>
+          <c:w val="0.11404435058078145"/>
+          <c:h val="0.42647211939955598"/>
         </c:manualLayout>
       </c:layout>
       <c:spPr>
@@ -4100,7 +4078,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter alignWithMargins="0"/>
-    <c:pageMargins b="1" l="0.75000000000000022" r="0.75000000000000022" t="1" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1" l="0.75000000000000033" r="0.75000000000000033" t="1" header="0.5" footer="0.5"/>
     <c:pageSetup paperSize="9" orientation="landscape"/>
   </c:printSettings>
 </c:chartSpace>
@@ -4641,7 +4619,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B8" sqref="B8"/>
+      <selection pane="bottomLeft" activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -4692,7 +4670,7 @@
       <c r="A5" s="34">
         <v>1</v>
       </c>
-      <c r="B5" s="105" t="s">
+      <c r="B5" s="102" t="s">
         <v>109</v>
       </c>
       <c r="C5" s="34" t="s">
@@ -4709,14 +4687,14 @@
       <c r="A6" s="34">
         <v>2</v>
       </c>
-      <c r="B6" s="105" t="s">
+      <c r="B6" s="102" t="s">
         <v>110</v>
       </c>
       <c r="C6" s="34" t="s">
         <v>19</v>
       </c>
       <c r="D6" s="34">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="E6" s="34">
         <v>1</v>
@@ -4729,14 +4707,14 @@
       <c r="A7" s="34">
         <v>3</v>
       </c>
-      <c r="B7" s="105" t="s">
+      <c r="B7" s="102" t="s">
         <v>111</v>
       </c>
       <c r="C7" s="34" t="s">
         <v>19</v>
       </c>
       <c r="D7" s="34">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="E7" s="34">
         <v>2</v>
@@ -4808,46 +4786,46 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="G44:G52 C45:C46 A11:A52 G23:G41 B11:F44 A54:G163 B47:F52 G11:G21 A4:G10">
-    <cfRule type="expression" dxfId="32" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="29" priority="1" stopIfTrue="1">
       <formula>$C4="Done"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="31" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="28" priority="2" stopIfTrue="1">
       <formula>$C4="Ongoing"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="30" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="27" priority="3" stopIfTrue="1">
       <formula>$C4="Removed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G53">
-    <cfRule type="expression" dxfId="29" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="26" priority="4" stopIfTrue="1">
       <formula>$C43="Done"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="28" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="25" priority="5" stopIfTrue="1">
       <formula>$C43="Ongoing"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="27" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="24" priority="6" stopIfTrue="1">
       <formula>$C43="Removed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G42:G43">
-    <cfRule type="expression" dxfId="26" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="23" priority="7" stopIfTrue="1">
       <formula>#REF!="Done"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="25" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="22" priority="8" stopIfTrue="1">
       <formula>#REF!="Ongoing"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="24" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="21" priority="9" stopIfTrue="1">
       <formula>#REF!="Removed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G22">
-    <cfRule type="expression" dxfId="23" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="20" priority="10" stopIfTrue="1">
       <formula>#REF!="Done"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="22" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="19" priority="11" stopIfTrue="1">
       <formula>#REF!="Ongoing"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="21" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="18" priority="12" stopIfTrue="1">
       <formula>#REF!="Removed"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4934,7 +4912,7 @@
       </c>
       <c r="E4" s="22">
         <f>IF(A4="","",SUMIF(I$16:I$30,'Release Plan'!A4,E$16:E$30))</f>
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="49"/>
@@ -5115,7 +5093,7 @@
       </c>
       <c r="E16" s="22">
         <f>IF(A16="","",SUMIF('Product Backlog'!E$5:E$103,'Release Plan'!A16,'Product Backlog'!D$5:D$103))</f>
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="F16" s="4" t="s">
         <v>19</v>
@@ -5145,7 +5123,7 @@
       </c>
       <c r="E17" s="22">
         <f>IF(A17="","",SUMIF('Product Backlog'!E$5:E$103,'Release Plan'!A17,'Product Backlog'!D$5:D$103))</f>
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="F17" s="4" t="s">
         <v>19</v>
@@ -5534,29 +5512,29 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="G4:H10 E31 E5:E10 A4:D10">
-    <cfRule type="expression" dxfId="20" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="17" priority="1" stopIfTrue="1">
       <formula>$F4="Planned"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="19" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="16" priority="2" stopIfTrue="1">
       <formula>$F4="Ongoing"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F4:F10 F16:F30">
-    <cfRule type="expression" dxfId="18" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="15" priority="3" stopIfTrue="1">
       <formula>$F4="Planned"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="17" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="14" priority="4" stopIfTrue="1">
       <formula>$F4="Ongoing"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="5" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="5" stopIfTrue="1" operator="equal">
       <formula>"Unplanned"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4 G16:H30 A16:E30">
-    <cfRule type="expression" dxfId="15" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="12" priority="6" stopIfTrue="1">
       <formula>OR($F4="Planned",$F4="Unplanned")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="11" priority="7" stopIfTrue="1">
       <formula>$F4="Ongoing"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5670,11 +5648,11 @@
       </c>
     </row>
     <row r="8" spans="1:26">
-      <c r="A8" s="102">
+      <c r="A8" s="103">
         <f>D$4</f>
         <v>3</v>
       </c>
-      <c r="B8" s="102"/>
+      <c r="B8" s="103"/>
       <c r="D8" s="58">
         <f ca="1">IF(D28="","",AVERAGE(OFFSET(D27,TrendOffset,0,SprintsInTrend,1)))</f>
         <v>25</v>
@@ -5786,11 +5764,11 @@
       </c>
     </row>
     <row r="18" spans="1:17">
-      <c r="A18" s="102">
+      <c r="A18" s="103">
         <f>D$4</f>
         <v>3</v>
       </c>
-      <c r="B18" s="102"/>
+      <c r="B18" s="103"/>
       <c r="D18" s="59">
         <f ca="1">IF(D8="","",IF(LastRealized="",ROUNDUP(LastPlanned/D8,0)+SprintCount-1,ROUNDUP((LastPlanned-LastRealized)/D8+SprintCount,0)))</f>
         <v>6</v>
@@ -5865,22 +5843,22 @@
       </c>
     </row>
     <row r="26" spans="1:17" ht="12.75" customHeight="1">
-      <c r="F26" s="104" t="s">
+      <c r="F26" s="105" t="s">
         <v>24</v>
       </c>
-      <c r="G26" s="104"/>
-      <c r="H26" s="104"/>
-      <c r="I26" s="104"/>
-      <c r="J26" s="104"/>
-      <c r="K26" s="104"/>
-      <c r="L26" s="104"/>
-      <c r="M26" s="104"/>
-      <c r="N26" s="104"/>
-      <c r="O26" s="104" t="s">
+      <c r="G26" s="105"/>
+      <c r="H26" s="105"/>
+      <c r="I26" s="105"/>
+      <c r="J26" s="105"/>
+      <c r="K26" s="105"/>
+      <c r="L26" s="105"/>
+      <c r="M26" s="105"/>
+      <c r="N26" s="105"/>
+      <c r="O26" s="105" t="s">
         <v>69</v>
       </c>
-      <c r="P26" s="104"/>
-      <c r="Q26" s="104"/>
+      <c r="P26" s="105"/>
+      <c r="Q26" s="105"/>
     </row>
     <row r="27" spans="1:17" s="3" customFormat="1" ht="26.25" thickBot="1">
       <c r="A27" s="60" t="s">
@@ -5901,10 +5879,10 @@
       <c r="F27" s="63" t="s">
         <v>35</v>
       </c>
-      <c r="G27" s="103" t="s">
+      <c r="G27" s="104" t="s">
         <v>38</v>
       </c>
-      <c r="H27" s="103"/>
+      <c r="H27" s="104"/>
       <c r="I27" s="63" t="s">
         <v>36</v>
       </c>
@@ -7358,13 +7336,13 @@
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="K27:N27 A27:G27 F26 I27 O26:O27 P27:Q27">
-    <cfRule type="expression" dxfId="13" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="10" priority="1" stopIfTrue="1">
       <formula>$D26="Done"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="9" priority="2" stopIfTrue="1">
       <formula>$D26="Ongoing"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="8" priority="3" stopIfTrue="1">
       <formula>$D26="Removed"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9113,10 +9091,10 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="A15:AD58">
-    <cfRule type="expression" dxfId="10" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="7" priority="1" stopIfTrue="1">
       <formula>$D15="Done"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="6" priority="2" stopIfTrue="1">
       <formula>$D15="Ongoing"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10397,7 +10375,7 @@
         <v/>
       </c>
       <c r="AC52" s="34" t="str">
-        <f t="shared" ref="AC52:AD70" si="8">IF(OR(AC$14="",$E52=""),"",AB52)</f>
+        <f t="shared" ref="AC52:AD63" si="8">IF(OR(AC$14="",$E52=""),"",AB52)</f>
         <v/>
       </c>
       <c r="AD52" s="34" t="str">
@@ -10868,10 +10846,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A15:AD58">
-    <cfRule type="expression" dxfId="4" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="5" priority="1" stopIfTrue="1">
       <formula>$D15="Done"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="4" priority="2" stopIfTrue="1">
       <formula>$D15="Ongoing"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -12544,18 +12522,18 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="A19:AD58 J15:AD18">
-    <cfRule type="expression" dxfId="8" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="3" priority="1" stopIfTrue="1">
       <formula>$D15="Done"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="2" priority="2" stopIfTrue="1">
       <formula>$D15="Ongoing"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A15:I18">
-    <cfRule type="expression" dxfId="6" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="1" priority="3" stopIfTrue="1">
       <formula>$D15="Done"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="0" priority="4" stopIfTrue="1">
       <formula>$D15="Ongoing"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>